<commit_message>
that was the excel file
</commit_message>
<xml_diff>
--- a/Pranaav-UIT2201-ex-05/Sorting_algorithm_analysis.xlsx
+++ b/Pranaav-UIT2201-ex-05/Sorting_algorithm_analysis.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="31">
   <si>
     <t>Sorting Algorithms</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Best Case</t>
   </si>
   <si>
-    <t>No of elements 10</t>
-  </si>
-  <si>
     <t>Worst Case</t>
   </si>
   <si>
@@ -96,6 +93,36 @@
   </si>
   <si>
     <t>Selection Sorting</t>
+  </si>
+  <si>
+    <t>78.246298 sec</t>
+  </si>
+  <si>
+    <t>No of elements 10000</t>
+  </si>
+  <si>
+    <t>0.0 sec</t>
+  </si>
+  <si>
+    <t>0.00100159 sec</t>
+  </si>
+  <si>
+    <t>7.496468 sec</t>
+  </si>
+  <si>
+    <t>22.779952 sec</t>
+  </si>
+  <si>
+    <t>0.084 sec</t>
+  </si>
+  <si>
+    <t>16.894478 sec</t>
+  </si>
+  <si>
+    <t>0.163999 sec</t>
+  </si>
+  <si>
+    <t>0.00099945sec</t>
   </si>
 </sst>
 </file>
@@ -193,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -207,10 +234,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -222,7 +249,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -240,60 +270,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>588816</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>92363</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>2308</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>161636</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9B927A6A-7A42-60B6-F154-C7BEF684E038}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="34165" t="31162" b="5988"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12318998" y="646545"/>
-          <a:ext cx="8589819" cy="4398819"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -585,7 +561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -593,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -604,37 +580,38 @@
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="27.21875" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1"/>
@@ -651,20 +628,20 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="20.399999999999999">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2"/>
@@ -681,22 +658,22 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="20.399999999999999">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="11" t="s">
@@ -790,8 +767,8 @@
       <c r="C11" s="3">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
+      <c r="D11" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="E11" s="11">
         <f>B11/A11</f>
@@ -824,8 +801,8 @@
       <c r="C12" s="3">
         <v>2165</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
+      <c r="D12" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" ref="E12:E14" si="0">B12/A12</f>
@@ -858,8 +835,8 @@
       <c r="C13" s="3">
         <v>247415</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>11</v>
+      <c r="D13" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
@@ -892,8 +869,8 @@
       <c r="C14" s="3">
         <v>24895445</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
+      <c r="D14" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
@@ -917,11 +894,17 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="17.399999999999999">
-      <c r="A15" s="14">
+      <c r="A15" s="10">
         <v>20000</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="10">
         <v>200010000</v>
+      </c>
+      <c r="C15" s="10">
+        <v>100113808</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="E15" s="11">
         <f t="shared" ref="E15" si="4">B15/A15</f>
@@ -950,7 +933,7 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>6</v>
@@ -962,51 +945,51 @@
     </row>
     <row r="17" spans="1:12" ht="17.399999999999999">
       <c r="A17" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="3">
-        <v>45</v>
+        <v>49995000</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17.399999999999999">
       <c r="A18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="8">
-        <v>11</v>
+        <v>25382922</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.399999999999999">
-      <c r="A22" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
+      <c r="A22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2"/>
@@ -1023,22 +1006,22 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" ht="20.399999999999999">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="11" t="s">
@@ -1130,10 +1113,10 @@
         <v>45</v>
       </c>
       <c r="C29" s="3">
-        <v>15</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="E29" s="11">
         <f>B29/A29</f>
@@ -1164,10 +1147,10 @@
         <v>4950</v>
       </c>
       <c r="C30" s="3">
-        <v>2165</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>10</v>
+        <v>94</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="E30" s="11">
         <f t="shared" ref="E30:E31" si="8">B30/A30</f>
@@ -1175,12 +1158,12 @@
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="12">
-        <f t="shared" ref="G30:G32" si="9">E30/A30</f>
+        <f t="shared" ref="G30:G31" si="9">E30/A30</f>
         <v>0.495</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="11">
-        <f t="shared" ref="I30:I32" si="10">G30/A30</f>
+        <f t="shared" ref="I30:I31" si="10">G30/A30</f>
         <v>4.9499999999999995E-3</v>
       </c>
       <c r="J30" s="11"/>
@@ -1198,10 +1181,10 @@
         <v>499500</v>
       </c>
       <c r="C31" s="3">
-        <v>247415</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>11</v>
+        <v>993</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E31" s="11">
         <f t="shared" si="8"/>
@@ -1232,10 +1215,10 @@
         <v>49995000</v>
       </c>
       <c r="C32" s="3">
-        <v>24895445</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>12</v>
+        <v>9987</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="E32" s="11">
         <f>B32/A32</f>
@@ -1259,11 +1242,17 @@
       <c r="L32" s="11"/>
     </row>
     <row r="33" spans="1:12" ht="17.399999999999999">
-      <c r="A33" s="14">
+      <c r="A33" s="10">
         <v>20000</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="10">
         <v>200010000</v>
+      </c>
+      <c r="C33" s="10">
+        <v>19977</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="E33" s="11">
         <f>B33/A33</f>
@@ -1292,7 +1281,7 @@
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>6</v>
@@ -1304,85 +1293,386 @@
     </row>
     <row r="36" spans="1:12" ht="17.399999999999999">
       <c r="A36" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="3">
-        <v>45</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="17.399999999999999">
       <c r="A37" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="8">
+        <v>9990</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="16.5" customHeight="1"/>
+    <row r="41" spans="1:12" ht="20.399999999999999">
+      <c r="A41" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" ht="20.399999999999999">
+      <c r="A43" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+    </row>
+    <row r="46" spans="1:12" ht="17.399999999999999">
+      <c r="A46" s="9"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="12"/>
+      <c r="I46" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L46" s="11"/>
+    </row>
+    <row r="47" spans="1:12" ht="17.399999999999999">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="11"/>
+      <c r="G47" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="12"/>
+      <c r="I47" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L47" s="11"/>
+    </row>
+    <row r="48" spans="1:12" ht="17.399999999999999">
+      <c r="A48" s="9">
+        <v>10</v>
+      </c>
+      <c r="B48" s="9">
+        <v>45</v>
+      </c>
+      <c r="C48" s="9">
+        <v>15</v>
+      </c>
+      <c r="D48" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="16.5" customHeight="1"/>
+      <c r="E48" s="11">
+        <f>B48/A48</f>
+        <v>4.5</v>
+      </c>
+      <c r="F48" s="11"/>
+      <c r="G48" s="12">
+        <f>E48/A48</f>
+        <v>0.45</v>
+      </c>
+      <c r="H48" s="12"/>
+      <c r="I48" s="11">
+        <f>G48/A48</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11">
+        <f>B48/(LOG(A48,2)*A48)</f>
+        <v>1.3546349804879154</v>
+      </c>
+      <c r="L48" s="11"/>
+    </row>
+    <row r="49" spans="1:12" ht="17.399999999999999">
+      <c r="A49" s="9">
+        <v>100</v>
+      </c>
+      <c r="B49" s="9">
+        <v>4950</v>
+      </c>
+      <c r="C49" s="9">
+        <v>2165</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" ref="E49:E50" si="13">B49/A49</f>
+        <v>49.5</v>
+      </c>
+      <c r="F49" s="11"/>
+      <c r="G49" s="12">
+        <f t="shared" ref="G49:G50" si="14">E49/A49</f>
+        <v>0.495</v>
+      </c>
+      <c r="H49" s="12"/>
+      <c r="I49" s="11">
+        <f t="shared" ref="I49:I50" si="15">G49/A49</f>
+        <v>4.9499999999999995E-3</v>
+      </c>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11">
+        <f t="shared" ref="K49:K52" si="16">B49/(LOG(A49,2)*A49)</f>
+        <v>7.4504923926835342</v>
+      </c>
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="1:12" ht="17.399999999999999">
+      <c r="A50" s="9">
+        <v>1000</v>
+      </c>
+      <c r="B50" s="9">
+        <v>499500</v>
+      </c>
+      <c r="C50" s="9">
+        <v>247415</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="11">
+        <f t="shared" si="13"/>
+        <v>499.5</v>
+      </c>
+      <c r="F50" s="11"/>
+      <c r="G50" s="12">
+        <f t="shared" si="14"/>
+        <v>0.4995</v>
+      </c>
+      <c r="H50" s="12"/>
+      <c r="I50" s="11">
+        <f t="shared" si="15"/>
+        <v>4.9950000000000005E-4</v>
+      </c>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11">
+        <f t="shared" si="16"/>
+        <v>50.121494278052865</v>
+      </c>
+      <c r="L50" s="11"/>
+    </row>
+    <row r="51" spans="1:12" ht="17.399999999999999">
+      <c r="A51" s="9">
+        <v>10000</v>
+      </c>
+      <c r="B51" s="9">
+        <v>49995000</v>
+      </c>
+      <c r="C51" s="9">
+        <v>24895445</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="11">
+        <f>B51/A51</f>
+        <v>4999.5</v>
+      </c>
+      <c r="F51" s="11"/>
+      <c r="G51" s="12">
+        <f>E51/A51</f>
+        <v>0.49995000000000001</v>
+      </c>
+      <c r="H51" s="12"/>
+      <c r="I51" s="11">
+        <f>G51/A51</f>
+        <v>4.9994999999999998E-5</v>
+      </c>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11">
+        <f t="shared" si="16"/>
+        <v>376.2498658305185</v>
+      </c>
+      <c r="L51" s="11"/>
+    </row>
+    <row r="52" spans="1:12" ht="17.399999999999999">
+      <c r="A52" s="10">
+        <v>20000</v>
+      </c>
+      <c r="B52" s="10">
+        <v>200010000</v>
+      </c>
+      <c r="E52" s="11">
+        <f>B52/A52</f>
+        <v>10000.5</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="12">
+        <f>E52/A52</f>
+        <v>0.50002500000000005</v>
+      </c>
+      <c r="H52" s="12"/>
+      <c r="I52" s="11">
+        <f>G52/A52</f>
+        <v>2.5001250000000004E-5</v>
+      </c>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11">
+        <f t="shared" si="16"/>
+        <v>699.93710219937645</v>
+      </c>
+      <c r="L52" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="79">
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:L24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:L26"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
+  <mergeCells count="115">
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="E43:L43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:L45"/>
+    <mergeCell ref="A1:L2"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:L8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K10:L10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="A22:L22"/>
     <mergeCell ref="E12:F12"/>
@@ -1399,25 +1689,53 @@
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="A1:L2"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:L8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:L24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:L26"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished the excel file
</commit_message>
<xml_diff>
--- a/Pranaav-UIT2201-ex-05/Sorting_algorithm_analysis.xlsx
+++ b/Pranaav-UIT2201-ex-05/Sorting_algorithm_analysis.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="33">
   <si>
     <t>Sorting Algorithms</t>
   </si>
@@ -110,9 +110,6 @@
     <t>7.496468 sec</t>
   </si>
   <si>
-    <t>22.779952 sec</t>
-  </si>
-  <si>
     <t>0.084 sec</t>
   </si>
   <si>
@@ -123,6 +120,15 @@
   </si>
   <si>
     <t>0.00099945sec</t>
+  </si>
+  <si>
+    <t>29.2367415 sec</t>
+  </si>
+  <si>
+    <t>9.05528 sec</t>
+  </si>
+  <si>
+    <t>Insertion Sorting</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +184,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -243,16 +255,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -561,7 +579,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -584,34 +602,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1"/>
@@ -628,20 +646,20 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="20.399999999999999">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2"/>
@@ -658,104 +676,104 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="20.399999999999999">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="17.399999999999999">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="11" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11" t="s">
+      <c r="J9" s="13"/>
+      <c r="K9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="11"/>
+      <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" ht="33" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="11" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11" t="s">
+      <c r="J10" s="13"/>
+      <c r="K10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L10" s="11"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" ht="28.5" customHeight="1">
       <c r="A11" s="3">
@@ -770,26 +788,26 @@
       <c r="D11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="13">
         <f>B11/A11</f>
         <v>7.7</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12">
+      <c r="F11" s="13"/>
+      <c r="G11" s="14">
         <f>E11/A11</f>
         <v>0.77</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="11">
+      <c r="H11" s="14"/>
+      <c r="I11" s="13">
         <f>G11/A11</f>
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13">
         <f>B11/(LOG(A11,2)*A11)</f>
         <v>2.3179309666126553</v>
       </c>
-      <c r="L11" s="11"/>
+      <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="3">
@@ -802,28 +820,28 @@
         <v>2165</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="11">
+        <v>29</v>
+      </c>
+      <c r="E12" s="13">
         <f t="shared" ref="E12:E14" si="0">B12/A12</f>
         <v>50.5</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12">
+      <c r="F12" s="13"/>
+      <c r="G12" s="14">
         <f t="shared" ref="G12:G14" si="1">E12/A12</f>
         <v>0.505</v>
       </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="11">
+      <c r="H12" s="14"/>
+      <c r="I12" s="13">
         <f t="shared" ref="I12:I14" si="2">G12/A12</f>
         <v>5.0499999999999998E-3</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11">
+      <c r="J12" s="13"/>
+      <c r="K12" s="13">
         <f t="shared" ref="K12:K14" si="3">B12/(LOG(A12,2)*A12)</f>
         <v>7.6010073905155249</v>
       </c>
-      <c r="L12" s="11"/>
+      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="29.25" customHeight="1">
       <c r="A13" s="3">
@@ -836,28 +854,28 @@
         <v>247415</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="11">
+        <v>28</v>
+      </c>
+      <c r="E13" s="13">
         <f t="shared" si="0"/>
         <v>500.5</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12">
+      <c r="F13" s="13"/>
+      <c r="G13" s="14">
         <f t="shared" si="1"/>
         <v>0.50049999999999994</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="11">
+      <c r="H13" s="14"/>
+      <c r="I13" s="13">
         <f t="shared" si="2"/>
         <v>5.0049999999999997E-4</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11">
+      <c r="J13" s="13"/>
+      <c r="K13" s="13">
         <f t="shared" si="3"/>
         <v>50.221837609940856</v>
       </c>
-      <c r="L13" s="11"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" ht="28.5" customHeight="1">
       <c r="A14" s="3">
@@ -870,30 +888,30 @@
         <v>24895445</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="11">
+        <v>27</v>
+      </c>
+      <c r="E14" s="13">
         <f t="shared" si="0"/>
         <v>5000.5</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12">
+      <c r="F14" s="13"/>
+      <c r="G14" s="14">
         <f t="shared" si="1"/>
         <v>0.50004999999999999</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="11">
+      <c r="H14" s="14"/>
+      <c r="I14" s="13">
         <f t="shared" si="2"/>
         <v>5.0005E-5</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11">
+      <c r="J14" s="13"/>
+      <c r="K14" s="13">
         <f t="shared" si="3"/>
         <v>376.32512332943446</v>
       </c>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" ht="17.399999999999999">
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" ht="18" customHeight="1">
       <c r="A15" s="10">
         <v>20000</v>
       </c>
@@ -906,46 +924,30 @@
       <c r="D15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="13">
         <f t="shared" ref="E15" si="4">B15/A15</f>
         <v>10000.5</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12">
+      <c r="F15" s="13"/>
+      <c r="G15" s="14">
         <f t="shared" ref="G15" si="5">E15/A15</f>
         <v>0.50002500000000005</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="11">
+      <c r="H15" s="14"/>
+      <c r="I15" s="13">
         <f t="shared" ref="I15" si="6">G15/A15</f>
         <v>2.5001250000000004E-5</v>
       </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11">
+      <c r="J15" s="13"/>
+      <c r="K15" s="13">
         <f t="shared" ref="K15" si="7">B15/(LOG(A15,2)*A15)</f>
         <v>699.93710219937645</v>
       </c>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="16" spans="1:12" ht="17.399999999999999">
-      <c r="A16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
+      <c r="L15" s="13"/>
     </row>
     <row r="17" spans="1:12" ht="17.399999999999999">
       <c r="A17" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
@@ -956,40 +958,56 @@
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17.399999999999999">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3">
         <v>49995000</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="17.399999999999999">
-      <c r="A18" s="6" t="s">
+    <row r="19" spans="1:12" ht="17.399999999999999">
+      <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8">
+      <c r="E19" s="7"/>
+      <c r="F19" s="8">
         <v>25382922</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="20.399999999999999">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2"/>
@@ -1006,104 +1024,104 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" ht="20.399999999999999">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14" t="s">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
     </row>
     <row r="26" spans="1:12" ht="33" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" ht="17.399999999999999">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="12" t="s">
+      <c r="F27" s="13"/>
+      <c r="G27" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="11" t="s">
+      <c r="H27" s="14"/>
+      <c r="I27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11" t="s">
+      <c r="J27" s="13"/>
+      <c r="K27" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L27" s="11"/>
+      <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" ht="30.75" customHeight="1">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="12" t="s">
+      <c r="F28" s="13"/>
+      <c r="G28" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H28" s="12"/>
-      <c r="I28" s="11" t="s">
+      <c r="H28" s="14"/>
+      <c r="I28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11" t="s">
+      <c r="J28" s="13"/>
+      <c r="K28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L28" s="11"/>
+      <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" ht="27.75" customHeight="1">
       <c r="A29" s="3">
@@ -1118,26 +1136,26 @@
       <c r="D29" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="13">
         <f>B29/A29</f>
         <v>4.5</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="12">
+      <c r="F29" s="13"/>
+      <c r="G29" s="14">
         <f>E29/A29</f>
         <v>0.45</v>
       </c>
-      <c r="H29" s="12"/>
-      <c r="I29" s="11">
+      <c r="H29" s="14"/>
+      <c r="I29" s="13">
         <f>G29/A29</f>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11">
+      <c r="J29" s="13"/>
+      <c r="K29" s="13">
         <f>B29/(LOG(A29,2)*A29)</f>
         <v>1.3546349804879154</v>
       </c>
-      <c r="L29" s="11"/>
+      <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" ht="28.5" customHeight="1">
       <c r="A30" s="3">
@@ -1152,26 +1170,26 @@
       <c r="D30" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="13">
         <f t="shared" ref="E30:E31" si="8">B30/A30</f>
         <v>49.5</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="12">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14">
         <f t="shared" ref="G30:G31" si="9">E30/A30</f>
         <v>0.495</v>
       </c>
-      <c r="H30" s="12"/>
-      <c r="I30" s="11">
+      <c r="H30" s="14"/>
+      <c r="I30" s="13">
         <f t="shared" ref="I30:I31" si="10">G30/A30</f>
         <v>4.9499999999999995E-3</v>
       </c>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11">
+      <c r="J30" s="13"/>
+      <c r="K30" s="13">
         <f t="shared" ref="K30:K32" si="11">B30/(LOG(A30,2)*A30)</f>
         <v>7.4504923926835342</v>
       </c>
-      <c r="L30" s="11"/>
+      <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" ht="28.5" customHeight="1">
       <c r="A31" s="3">
@@ -1184,28 +1202,28 @@
         <v>993</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="11">
+        <v>26</v>
+      </c>
+      <c r="E31" s="13">
         <f t="shared" si="8"/>
         <v>499.5</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="12">
+      <c r="F31" s="13"/>
+      <c r="G31" s="14">
         <f t="shared" si="9"/>
         <v>0.4995</v>
       </c>
-      <c r="H31" s="12"/>
-      <c r="I31" s="11">
+      <c r="H31" s="14"/>
+      <c r="I31" s="13">
         <f t="shared" si="10"/>
         <v>4.9950000000000005E-4</v>
       </c>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11">
+      <c r="J31" s="13"/>
+      <c r="K31" s="13">
         <f t="shared" si="11"/>
         <v>50.121494278052865</v>
       </c>
-      <c r="L31" s="11"/>
+      <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="3">
@@ -1220,26 +1238,26 @@
       <c r="D32" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E32" s="13">
         <f>B32/A32</f>
         <v>4999.5</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="12">
+      <c r="F32" s="13"/>
+      <c r="G32" s="14">
         <f>E32/A32</f>
         <v>0.49995000000000001</v>
       </c>
-      <c r="H32" s="12"/>
-      <c r="I32" s="11">
+      <c r="H32" s="14"/>
+      <c r="I32" s="13">
         <f>G32/A32</f>
         <v>4.9994999999999998E-5</v>
       </c>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11">
+      <c r="J32" s="13"/>
+      <c r="K32" s="13">
         <f t="shared" si="11"/>
         <v>376.2498658305185</v>
       </c>
-      <c r="L32" s="11"/>
+      <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="17.399999999999999">
       <c r="A33" s="10">
@@ -1252,93 +1270,93 @@
         <v>19977</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="11">
+        <v>30</v>
+      </c>
+      <c r="E33" s="13">
         <f>B33/A33</f>
         <v>10000.5</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="12">
+      <c r="F33" s="13"/>
+      <c r="G33" s="14">
         <f>E33/A33</f>
         <v>0.50002500000000005</v>
       </c>
-      <c r="H33" s="12"/>
-      <c r="I33" s="11">
+      <c r="H33" s="14"/>
+      <c r="I33" s="13">
         <f>G33/A33</f>
         <v>2.5001250000000004E-5</v>
       </c>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11">
+      <c r="J33" s="13"/>
+      <c r="K33" s="13">
         <f t="shared" ref="K33" si="12">B33/(LOG(A33,2)*A33)</f>
         <v>699.93710219937645</v>
       </c>
-      <c r="L33" s="11"/>
+      <c r="L33" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="17.399999999999999">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="11"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="11"/>
+      <c r="E35" s="13"/>
       <c r="F35" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="17.399999999999999">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="11"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="11"/>
+      <c r="E36" s="13"/>
       <c r="F36" s="3">
         <v>5000</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="17.399999999999999">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="16"/>
       <c r="C37" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="13"/>
+      <c r="E37" s="16"/>
       <c r="F37" s="8">
         <v>9990</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="16.5" customHeight="1"/>
     <row r="41" spans="1:12" ht="20.399999999999999">
-      <c r="A41" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
+      <c r="A41" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="2"/>
@@ -1355,111 +1373,111 @@
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="1:12" ht="20.399999999999999">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14" t="s">
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="17.399999999999999">
       <c r="A46" s="9"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="12" t="s">
+      <c r="F46" s="13"/>
+      <c r="G46" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H46" s="12"/>
-      <c r="I46" s="11" t="s">
+      <c r="H46" s="14"/>
+      <c r="I46" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11" t="s">
+      <c r="J46" s="13"/>
+      <c r="K46" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L46" s="11"/>
+      <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="17.399999999999999">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="12" t="s">
+      <c r="F47" s="13"/>
+      <c r="G47" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="12"/>
-      <c r="I47" s="11" t="s">
+      <c r="H47" s="14"/>
+      <c r="I47" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11" t="s">
+      <c r="J47" s="13"/>
+      <c r="K47" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L47" s="11"/>
+      <c r="L47" s="13"/>
     </row>
     <row r="48" spans="1:12" ht="17.399999999999999">
       <c r="A48" s="9">
         <v>10</v>
       </c>
-      <c r="B48" s="9">
-        <v>45</v>
+      <c r="B48" s="11">
+        <v>15</v>
       </c>
       <c r="C48" s="9">
         <v>15</v>
@@ -1467,33 +1485,33 @@
       <c r="D48" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="11">
+      <c r="E48" s="13">
         <f>B48/A48</f>
-        <v>4.5</v>
-      </c>
-      <c r="F48" s="11"/>
-      <c r="G48" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="F48" s="13"/>
+      <c r="G48" s="14">
         <f>E48/A48</f>
-        <v>0.45</v>
-      </c>
-      <c r="H48" s="12"/>
-      <c r="I48" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="H48" s="14"/>
+      <c r="I48" s="13">
         <f>G48/A48</f>
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13">
         <f>B48/(LOG(A48,2)*A48)</f>
-        <v>1.3546349804879154</v>
-      </c>
-      <c r="L48" s="11"/>
+        <v>0.45154499349597177</v>
+      </c>
+      <c r="L48" s="13"/>
     </row>
     <row r="49" spans="1:12" ht="17.399999999999999">
       <c r="A49" s="9">
         <v>100</v>
       </c>
-      <c r="B49" s="9">
-        <v>4950</v>
+      <c r="B49" s="11">
+        <v>2165</v>
       </c>
       <c r="C49" s="9">
         <v>2165</v>
@@ -1501,33 +1519,33 @@
       <c r="D49" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E49" s="11">
+      <c r="E49" s="13">
         <f t="shared" ref="E49:E50" si="13">B49/A49</f>
-        <v>49.5</v>
-      </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="12">
+        <v>21.65</v>
+      </c>
+      <c r="F49" s="13"/>
+      <c r="G49" s="14">
         <f t="shared" ref="G49:G50" si="14">E49/A49</f>
-        <v>0.495</v>
-      </c>
-      <c r="H49" s="12"/>
-      <c r="I49" s="11">
+        <v>0.2165</v>
+      </c>
+      <c r="H49" s="14"/>
+      <c r="I49" s="13">
         <f t="shared" ref="I49:I50" si="15">G49/A49</f>
-        <v>4.9499999999999995E-3</v>
-      </c>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11">
+        <v>2.1649999999999998E-3</v>
+      </c>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13">
         <f t="shared" ref="K49:K52" si="16">B49/(LOG(A49,2)*A49)</f>
-        <v>7.4504923926835342</v>
-      </c>
-      <c r="L49" s="11"/>
+        <v>3.2586497030625963</v>
+      </c>
+      <c r="L49" s="13"/>
     </row>
     <row r="50" spans="1:12" ht="17.399999999999999">
       <c r="A50" s="9">
         <v>1000</v>
       </c>
-      <c r="B50" s="9">
-        <v>499500</v>
+      <c r="B50" s="11">
+        <v>247415</v>
       </c>
       <c r="C50" s="9">
         <v>247415</v>
@@ -1535,33 +1553,33 @@
       <c r="D50" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E50" s="13">
         <f t="shared" si="13"/>
-        <v>499.5</v>
-      </c>
-      <c r="F50" s="11"/>
-      <c r="G50" s="12">
+        <v>247.41499999999999</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="14">
         <f t="shared" si="14"/>
-        <v>0.4995</v>
-      </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="11">
+        <v>0.247415</v>
+      </c>
+      <c r="H50" s="14"/>
+      <c r="I50" s="13">
         <f t="shared" si="15"/>
-        <v>4.9950000000000005E-4</v>
-      </c>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11">
+        <v>2.4741500000000002E-4</v>
+      </c>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13">
         <f t="shared" si="16"/>
-        <v>50.121494278052865</v>
-      </c>
-      <c r="L50" s="11"/>
+        <v>24.826445459067966</v>
+      </c>
+      <c r="L50" s="13"/>
     </row>
     <row r="51" spans="1:12" ht="17.399999999999999">
       <c r="A51" s="9">
         <v>10000</v>
       </c>
-      <c r="B51" s="9">
-        <v>49995000</v>
+      <c r="B51" s="11">
+        <v>24895445</v>
       </c>
       <c r="C51" s="9">
         <v>24895445</v>
@@ -1569,85 +1587,180 @@
       <c r="D51" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E51" s="13">
         <f>B51/A51</f>
-        <v>4999.5</v>
-      </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="12">
+        <v>2489.5445</v>
+      </c>
+      <c r="F51" s="13"/>
+      <c r="G51" s="14">
         <f>E51/A51</f>
-        <v>0.49995000000000001</v>
-      </c>
-      <c r="H51" s="12"/>
-      <c r="I51" s="11">
+        <v>0.24895444999999999</v>
+      </c>
+      <c r="H51" s="14"/>
+      <c r="I51" s="13">
         <f>G51/A51</f>
-        <v>4.9994999999999998E-5</v>
-      </c>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11">
+        <v>2.4895444999999999E-5</v>
+      </c>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13">
         <f t="shared" si="16"/>
-        <v>376.2498658305185</v>
-      </c>
-      <c r="L51" s="11"/>
+        <v>187.35689251007204</v>
+      </c>
+      <c r="L51" s="13"/>
     </row>
     <row r="52" spans="1:12" ht="17.399999999999999">
       <c r="A52" s="10">
         <v>20000</v>
       </c>
       <c r="B52" s="10">
-        <v>200010000</v>
-      </c>
-      <c r="E52" s="11">
+        <v>100078576</v>
+      </c>
+      <c r="C52" s="10">
+        <v>100078576</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" s="13">
         <f>B52/A52</f>
-        <v>10000.5</v>
-      </c>
-      <c r="F52" s="11"/>
-      <c r="G52" s="12">
+        <v>5003.9287999999997</v>
+      </c>
+      <c r="F52" s="13"/>
+      <c r="G52" s="14">
         <f>E52/A52</f>
-        <v>0.50002500000000005</v>
-      </c>
-      <c r="H52" s="12"/>
-      <c r="I52" s="11">
+        <v>0.25019643999999996</v>
+      </c>
+      <c r="H52" s="14"/>
+      <c r="I52" s="13">
         <f>G52/A52</f>
-        <v>2.5001250000000004E-5</v>
-      </c>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11">
+        <v>1.2509821999999999E-5</v>
+      </c>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13">
         <f t="shared" si="16"/>
-        <v>699.93710219937645</v>
-      </c>
-      <c r="L52" s="11"/>
+        <v>350.22603108684598</v>
+      </c>
+      <c r="L52" s="13"/>
+    </row>
+    <row r="54" spans="1:12" ht="17.399999999999999">
+      <c r="A54" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="13"/>
+      <c r="F54" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="17.399999999999999">
+      <c r="A55" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="13"/>
+      <c r="F55" s="11">
+        <v>49985001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="17.399999999999999">
+      <c r="A56" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="16"/>
+      <c r="F56" s="12">
+        <v>24931795</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="115">
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
+  <mergeCells count="121">
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:L24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:L26"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
     <mergeCell ref="A41:L41"/>
     <mergeCell ref="A43:D43"/>
     <mergeCell ref="E43:L43"/>
@@ -1672,69 +1785,34 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:L24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:L26"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="K51:L51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>